<commit_message>
Added photo of hole diameter image for Ledia 6f
</commit_message>
<xml_diff>
--- a/DI Comparison Chart.xlsx
+++ b/DI Comparison Chart.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\CI\PCBEquipmentCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melissa\Documents\CI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="25605" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="25610" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LDI Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="121">
   <si>
     <t>Machine</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Dainippon Screen</t>
+  </si>
+  <si>
+    <t>ledia_img_02E_holediameter.jpg</t>
   </si>
 </sst>
 </file>
@@ -881,23 +884,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.125" customWidth="1"/>
-    <col min="3" max="3" width="59.875" customWidth="1"/>
+    <col min="1" max="1" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.08203125" customWidth="1"/>
+    <col min="3" max="3" width="59.83203125" customWidth="1"/>
     <col min="4" max="4" width="77.75" customWidth="1"/>
     <col min="5" max="5" width="124.25" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="133.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="103.625" customWidth="1"/>
+    <col min="8" max="8" width="103.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -973,7 +976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>117</v>
       </c>
@@ -988,7 +991,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1368,7 +1371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="63" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="62" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1406,7 +1409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1444,7 +1447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="110.25" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
@@ -1593,13 +1596,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
       <c r="E20" t="s">
         <v>8</v>
       </c>
@@ -1625,7 +1631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -1663,7 +1669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -1739,7 +1745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -1777,7 +1783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="63" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:12" ht="62" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
@@ -1815,7 +1821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>70</v>
       </c>
@@ -1891,7 +1897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>75</v>
       </c>
@@ -1967,7 +1973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>76</v>
       </c>
@@ -2005,7 +2011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>78</v>
       </c>
@@ -2043,7 +2049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>79</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -2119,7 +2125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
@@ -2157,7 +2163,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>83</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>84</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -2271,7 +2277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
@@ -2332,9 +2338,9 @@
       <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -2342,7 +2348,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>112</v>
       </c>
@@ -2350,7 +2356,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
Updated Ledia model names
</commit_message>
<xml_diff>
--- a/DI Comparison Chart.xlsx
+++ b/DI Comparison Chart.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="121">
   <si>
     <t>Machine</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>SpeedLight 2D</t>
-  </si>
-  <si>
-    <t>Ledia 6F</t>
   </si>
   <si>
     <t>INPREX</t>
@@ -420,7 +417,11 @@
     <t>Dainippon Screen</t>
   </si>
   <si>
-    <t>ledia_img_02E_holediameter.jpg</t>
+    <t>Ledia</t>
+  </si>
+  <si>
+    <t>Ledia 6S (Standard Model)
+Ledia 6F (Fine Line Model)</t>
   </si>
 </sst>
 </file>
@@ -884,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -908,1411 +909,1408 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>93</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
       <c r="I5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
       <c r="I6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H10" s="3">
         <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="62" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
-      </c>
       <c r="H14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H16" t="s">
-        <v>45</v>
-      </c>
       <c r="I16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
         <v>91</v>
       </c>
-      <c r="D17" t="s">
-        <v>92</v>
-      </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>52</v>
       </c>
-      <c r="D19" t="s">
-        <v>53</v>
-      </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" t="s">
-        <v>56</v>
-      </c>
       <c r="I21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="62" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
         <v>63</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>64</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>66</v>
       </c>
-      <c r="G25" t="s">
-        <v>67</v>
-      </c>
       <c r="H25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
         <v>68</v>
       </c>
-      <c r="B26" t="s">
-        <v>69</v>
-      </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
         <v>70</v>
       </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>71</v>
       </c>
-      <c r="D27" t="s">
-        <v>72</v>
-      </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
         <v>96</v>
       </c>
-      <c r="E29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" t="s">
-        <v>97</v>
-      </c>
       <c r="H29" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
         <v>76</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
-        <v>77</v>
-      </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>81</v>
-      </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" t="s">
         <v>85</v>
       </c>
-      <c r="B37" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" t="s">
-        <v>86</v>
-      </c>
       <c r="I37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2342,23 +2340,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>